<commit_message>
progs filmes com ajax + alteracoes home
</commit_message>
<xml_diff>
--- a/cronograma_site.xlsx
+++ b/cronograma_site.xlsx
@@ -292,9 +292,6 @@
     <t>17 de agosto</t>
   </si>
   <si>
-    <t>submenu responsivo, criar seção Sobre</t>
-  </si>
-  <si>
     <t>links de acesso a cada seção</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>inicialmente, submenu home só com 'sobre', com link para pag de residencias</t>
+  </si>
+  <si>
+    <t>submenu responsivo, criar seção Sobre -- ELIMINAR SUBMENUS INTERNOS -- AJAX</t>
   </si>
 </sst>
 </file>
@@ -427,8 +427,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="67">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -543,7 +545,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="67">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -577,6 +579,7 @@
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -610,6 +613,7 @@
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1328,8 +1332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1337,7 +1341,7 @@
     <col min="1" max="1" width="27.6640625" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="56.33203125" style="22" customWidth="1"/>
+    <col min="5" max="5" width="71" style="22" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18">
@@ -1530,7 +1534,7 @@
       <c r="C19" s="15"/>
       <c r="D19" s="5"/>
       <c r="E19" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1541,7 +1545,7 @@
       <c r="C20" s="16"/>
       <c r="D20" s="5"/>
       <c r="E20" s="21" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1590,12 +1594,12 @@
       <c r="C25" s="16"/>
       <c r="D25" s="5"/>
       <c r="E25" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="16"/>
@@ -1698,10 +1702,10 @@
         <v>79</v>
       </c>
       <c r="B36" s="6"/>
-      <c r="C36" s="14"/>
+      <c r="C36" s="15"/>
       <c r="D36" s="5"/>
       <c r="E36" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:5">

</xml_diff>

<commit_message>
troca de idioma com ajax em pps
</commit_message>
<xml_diff>
--- a/cronograma_site.xlsx
+++ b/cronograma_site.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="103">
   <si>
     <t>Artistas participantes</t>
   </si>
@@ -312,6 +312,24 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>falta foto danilo</t>
+  </si>
+  <si>
+    <t>falta fotos curadores</t>
+  </si>
+  <si>
+    <t>falta foto artistas</t>
+  </si>
+  <si>
+    <t>falta links</t>
+  </si>
+  <si>
+    <t>falta imagem texto em ingles / fotos do local</t>
+  </si>
+  <si>
+    <t>nao existe??</t>
   </si>
 </sst>
 </file>
@@ -434,8 +452,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -552,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="73">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -587,6 +609,8 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -621,6 +645,8 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1337,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1386,7 +1412,9 @@
         <v>85</v>
       </c>
       <c r="C3" s="15"/>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5">
@@ -1397,7 +1425,9 @@
         <v>85</v>
       </c>
       <c r="C4" s="15"/>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5">
@@ -1408,7 +1438,9 @@
         <v>85</v>
       </c>
       <c r="C5" s="15"/>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E5" s="21"/>
     </row>
     <row r="6" spans="1:5">
@@ -1419,7 +1451,9 @@
         <v>85</v>
       </c>
       <c r="C6" s="15"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:5">
@@ -1495,83 +1529,91 @@
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="18" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="15"/>
-      <c r="D15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="18" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="15"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="18" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="15"/>
-      <c r="D17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="18" t="s">
-        <v>66</v>
+      <c r="A18" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="15"/>
       <c r="D18" s="5"/>
-      <c r="E18" s="21"/>
+      <c r="E18" s="21" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="18" t="s">
-        <v>1</v>
+      <c r="A19" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="E19" s="21" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>94</v>
-      </c>
+      <c r="A20" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>86</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="B21" s="6"/>
       <c r="C21" s="15"/>
       <c r="D21" s="5"/>
       <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="18" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="15"/>
@@ -1580,45 +1622,49 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="18" t="s">
-        <v>71</v>
+      <c r="A24" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="15"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="21"/>
+      <c r="E24" s="21" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
-        <v>72</v>
+      <c r="A25" s="18" t="s">
+        <v>92</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="16"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="21" t="s">
-        <v>93</v>
-      </c>
+      <c r="E25" s="21"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="16"/>
+        <v>84</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="15"/>
       <c r="D26" s="5"/>
       <c r="E26" s="21"/>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="18" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>87</v>
@@ -1629,7 +1675,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="18" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>87</v>
@@ -1640,49 +1686,47 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>87</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="B29" s="6"/>
       <c r="C29" s="15"/>
       <c r="D29" s="5"/>
       <c r="E29" s="21"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="18" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="15"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="21"/>
+      <c r="E30" s="21" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="18" t="s">
-        <v>76</v>
+      <c r="A31" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="21" t="s">
-        <v>82</v>
-      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="2" t="s">
-        <v>3</v>
+      <c r="A32" s="18" t="s">
+        <v>77</v>
       </c>
       <c r="B32" s="6"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="5" t="s">
-        <v>95</v>
-      </c>
+      <c r="C32" s="15"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="21"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="15"/>
@@ -1691,38 +1735,38 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="15"/>
+        <v>4</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="14"/>
       <c r="D34" s="5"/>
       <c r="E34" s="21"/>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C35" s="14"/>
+        <v>79</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="15"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="21"/>
+      <c r="E35" s="21" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="18" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B36" s="6"/>
       <c r="C36" s="15"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="21" t="s">
-        <v>91</v>
-      </c>
+      <c r="E36" s="21"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="18" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B37" s="6"/>
       <c r="C37" s="15"/>
@@ -1730,22 +1774,13 @@
       <c r="E37" s="21"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="21"/>
+      <c r="A38" s="2"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2"/>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>